<commit_message>
Added Competitor Performance Dashboard
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w1mug\Desktop\naga\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B949504F-4AA3-4E6E-8759-C7D9BB7B4AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D3E2B0-F910-4CCA-860E-F77FF1F5F6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Products</t>
   </si>
@@ -48,41 +48,47 @@
     <t>Gulab Jamun Mix</t>
   </si>
   <si>
-    <t>Ragi Flour</t>
-  </si>
-  <si>
-    <t>Ragi Semiya</t>
-  </si>
-  <si>
-    <t>Rusk</t>
-  </si>
-  <si>
-    <t>Nandi</t>
-  </si>
-  <si>
-    <t>Local Brand</t>
-  </si>
-  <si>
-    <t>Local Brand, Aachi, MTR</t>
-  </si>
-  <si>
-    <t>Sakthi</t>
-  </si>
-  <si>
-    <t>Anil</t>
-  </si>
-  <si>
-    <t>Britannia</t>
-  </si>
-  <si>
-    <t>Bajji Bonda Mix</t>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Category: Price Concern / Discount Concern / Product Variety / Product Package Size / Other factors</t>
+  </si>
+  <si>
+    <t>Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi, Nandi</t>
+  </si>
+  <si>
+    <t>Price Concern, Price Concern,Price Concern,Price Concern,Price Concern,Price Concern,Price Concern,Price Concern,Price Concern,Price Concern, Discount Concern, Discount Concern, Discount Concern, Discount Concern, Discount Concern, Discount Concern, Discount Concern, Discount Concern, Discount Concern, Discount Concern, Price Concern,Price Concern,Price Concern,Price Concern,Price Concern,Price Concern,Price Concern,Price Concern,Price Concern,Price Concern</t>
+  </si>
+  <si>
+    <t>Local Brand, Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand,Local Brand</t>
+  </si>
+  <si>
+    <t>Product Package Size, Other factors, Product Variety, Product Package Size, Other factors, Product Variety,Product Package Size, Other factors, Product Variety,Product Package Size, Other factors, Product Variety,Product Package Size, Other factors, Product Variety,Product Package Size, Other factors, Product Variety,Product Package Size, Other factors, Product Variety,Product Package Size, Other factors, Product Variety,Product Package Size, Other factors,Other factors, Other factors, Other factors, Other factors</t>
+  </si>
+  <si>
+    <t>Local Brand, Local Brand, Local Brand, Local Brand, Local Brand, Local Brand,Local Brand, Local Brand, Local Brand, Local Brand</t>
+  </si>
+  <si>
+    <t>Aachi, Aachi, Aachi, Aachi, Aachi, Aachi, Aachi, Aachi, Aachi, Aachi, Aachi, Aachi, Aachi, Aachi, Aachi</t>
+  </si>
+  <si>
+    <t>Price Concern, Other factors, Other factors, Other factors, Other factors,Price Concern, Other factors, Other factors, Price Concern, Other factors, Price Concern, Other factors, Price Concern, Other factors, Price Concern</t>
+  </si>
+  <si>
+    <t>Price Concern,Price Concern,Price Concern,Price Concern,Price Concern,Price Concern,Price Concern,Price Concern,Price Concern,Price Concern</t>
+  </si>
+  <si>
+    <t>MTR, MTR, MTR, MTR, MTR, MTR, MTR, MTR, MTR, MTR,MTR,MTR,MTR,MTR,MTR,MTR,MTR,MTR,MTR,MTR,</t>
+  </si>
+  <si>
+    <t>Other factors, Product Package Size, Other factors, Product Package Size, Other factors, Other factors, Other factors, Product Package Size, Other factors, Other factors, Other factors, Product Package Size, Other factors, Product Package Size, Other factors, Product Package Size, Other factors, Other factors, Product Package Size, Other factors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +103,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -119,10 +131,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -404,96 +431,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.21875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="83.5546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I18" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Product Performance Dashboard
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w1mug\Desktop\naga\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D3E2B0-F910-4CCA-860E-F77FF1F5F6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF2314D-036B-4E7D-A591-EF406647C962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>